<commit_message>
web planform corrected bug
</commit_message>
<xml_diff>
--- a/new_modules/Summary_2022-06-09_L1C.xlsx
+++ b/new_modules/Summary_2022-06-09_L1C.xlsx
@@ -441,19 +441,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.4533</v>
+        <v>-0.0413</v>
       </c>
       <c r="C2">
-        <v>0.4533</v>
+        <v>-0.0413</v>
       </c>
       <c r="D2">
-        <v>0.4932000041007996</v>
+        <v>-0.05119999870657921</v>
       </c>
       <c r="E2">
-        <v>0.8985999822616577</v>
+        <v>0.1909999996423721</v>
       </c>
       <c r="F2">
-        <v>0.1775999963283539</v>
+        <v>-0.05119999870657921</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -461,19 +461,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.5469000000000001</v>
+        <v>-0.0472</v>
       </c>
       <c r="C3">
-        <v>0.5469000000000001</v>
+        <v>-0.0472</v>
       </c>
       <c r="D3">
-        <v>0.5558999999999999</v>
+        <v>-0.0512</v>
       </c>
       <c r="E3">
-        <v>0.7870000004768372</v>
+        <v>0.1248999983072281</v>
       </c>
       <c r="F3">
-        <v>0.2027000039815903</v>
+        <v>-0.05119999870657921</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -481,19 +481,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.4713</v>
+        <v>-0.0508</v>
       </c>
       <c r="C4">
-        <v>0.4713</v>
+        <v>-0.0508</v>
       </c>
       <c r="D4">
-        <v>0.4714</v>
+        <v>-0.0512</v>
       </c>
       <c r="E4">
-        <v>0.7348999977111816</v>
+        <v>0.09380000084638596</v>
       </c>
       <c r="F4">
-        <v>0.2377000004053116</v>
+        <v>-0.05119999870657921</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -501,19 +501,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.3393</v>
+        <v>0.0522</v>
       </c>
       <c r="C5">
-        <v>0.3393</v>
+        <v>0.0522</v>
       </c>
       <c r="D5">
-        <v>0.3364</v>
+        <v>0.0644</v>
       </c>
       <c r="E5">
-        <v>0.671500027179718</v>
+        <v>0.2610999941825867</v>
       </c>
       <c r="F5">
-        <v>0.1578000038862228</v>
+        <v>-0.05119999870657921</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -521,19 +521,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.3332</v>
+        <v>0.06850000000000001</v>
       </c>
       <c r="C6">
-        <v>0.3332</v>
+        <v>0.06850000000000001</v>
       </c>
       <c r="D6">
-        <v>0.3249</v>
+        <v>0.0441</v>
       </c>
       <c r="E6">
-        <v>0.7124000191688538</v>
+        <v>0.3282999992370605</v>
       </c>
       <c r="F6">
-        <v>0.1907999962568283</v>
+        <v>-0.05119999870657921</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -541,19 +541,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.3281</v>
+        <v>0.06610000000000001</v>
       </c>
       <c r="C7">
-        <v>0.3281</v>
+        <v>0.06610000000000001</v>
       </c>
       <c r="D7">
-        <v>0.338699996471405</v>
+        <v>0.05990000069141388</v>
       </c>
       <c r="E7">
-        <v>0.4912000000476837</v>
+        <v>0.221000000834465</v>
       </c>
       <c r="F7">
-        <v>0.2133000046014786</v>
+        <v>-0.05119999870657921</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -561,19 +561,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.274</v>
+        <v>0.08790000000000001</v>
       </c>
       <c r="C8">
-        <v>0.274</v>
+        <v>0.08790000000000001</v>
       </c>
       <c r="D8">
-        <v>0.2634</v>
+        <v>0.08019999999999999</v>
       </c>
       <c r="E8">
-        <v>0.4535999894142151</v>
+        <v>0.221000000834465</v>
       </c>
       <c r="F8">
-        <v>0.2020000070333481</v>
+        <v>-0.05119999870657921</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
styled dataframe display mode
</commit_message>
<xml_diff>
--- a/new_modules/Summary_2022-06-09_L1C.xlsx
+++ b/new_modules/Summary_2022-06-09_L1C.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Загон</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>№7</t>
+  </si>
+  <si>
+    <t>Пастбище</t>
   </si>
 </sst>
 </file>
@@ -410,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,7 +444,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>-0.0413</v>
+        <v>-55.01340103149414</v>
       </c>
       <c r="C2">
         <v>-0.0413</v>
@@ -461,7 +464,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>-0.0472</v>
+        <v>-59.02640151977539</v>
       </c>
       <c r="C3">
         <v>-0.0472</v>
@@ -481,7 +484,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>-0.0508</v>
+        <v>-43.45640182495117</v>
       </c>
       <c r="C4">
         <v>-0.0508</v>
@@ -501,7 +504,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.0522</v>
+        <v>49.46620178222656</v>
       </c>
       <c r="C5">
         <v>0.0522</v>
@@ -521,7 +524,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.06850000000000001</v>
+        <v>86.60639953613281</v>
       </c>
       <c r="C6">
         <v>0.06850000000000001</v>
@@ -541,7 +544,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.06610000000000001</v>
+        <v>65.66690063476562</v>
       </c>
       <c r="C7">
         <v>0.06610000000000001</v>
@@ -561,7 +564,7 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.08790000000000001</v>
+        <v>98.10030364990234</v>
       </c>
       <c r="C8">
         <v>0.08790000000000001</v>
@@ -573,6 +576,26 @@
         <v>0.221000000834465</v>
       </c>
       <c r="F8">
+        <v>-0.05119999870657921</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>142.3435974121094</v>
+      </c>
+      <c r="C9">
+        <v>0.0182</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.3282999992370605</v>
+      </c>
+      <c r="F9">
         <v>-0.05119999870657921</v>
       </c>
     </row>

</xml_diff>

<commit_message>
normalization correction over dates
</commit_message>
<xml_diff>
--- a/new_modules/Summary_2022-06-09_L1C.xlsx
+++ b/new_modules/Summary_2022-06-09_L1C.xlsx
@@ -444,19 +444,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>-55.01340103149414</v>
+        <v>-144.9629974365234</v>
       </c>
       <c r="C2">
-        <v>-0.0413</v>
+        <v>-0.1087</v>
       </c>
       <c r="D2">
-        <v>-0.05119999870657921</v>
+        <v>-0.1348000019788742</v>
       </c>
       <c r="E2">
-        <v>0.1909999996423721</v>
+        <v>0.5033000111579895</v>
       </c>
       <c r="F2">
-        <v>-0.05119999870657921</v>
+        <v>-0.1348000019788742</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -464,19 +464,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>-59.02640151977539</v>
+        <v>-155.5372924804688</v>
       </c>
       <c r="C3">
-        <v>-0.0472</v>
+        <v>-0.1244</v>
       </c>
       <c r="D3">
-        <v>-0.0512</v>
+        <v>-0.1348</v>
       </c>
       <c r="E3">
-        <v>0.1248999983072281</v>
+        <v>0.3291000127792358</v>
       </c>
       <c r="F3">
-        <v>-0.05119999870657921</v>
+        <v>-0.1348000019788742</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -484,19 +484,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>-43.45640182495117</v>
+        <v>-114.5098037719727</v>
       </c>
       <c r="C4">
-        <v>-0.0508</v>
+        <v>-0.1338</v>
       </c>
       <c r="D4">
-        <v>-0.0512</v>
+        <v>-0.1348</v>
       </c>
       <c r="E4">
-        <v>0.09380000084638596</v>
+        <v>0.2471999973058701</v>
       </c>
       <c r="F4">
-        <v>-0.05119999870657921</v>
+        <v>-0.1348000019788742</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -504,19 +504,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>49.46620178222656</v>
+        <v>130.3462066650391</v>
       </c>
       <c r="C5">
-        <v>0.0522</v>
+        <v>0.1375</v>
       </c>
       <c r="D5">
-        <v>0.0644</v>
+        <v>0.1698</v>
       </c>
       <c r="E5">
-        <v>0.2610999941825867</v>
+        <v>0.6880000233650208</v>
       </c>
       <c r="F5">
-        <v>-0.05119999870657921</v>
+        <v>-0.1348000019788742</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -524,19 +524,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>86.60639953613281</v>
+        <v>228.21240234375</v>
       </c>
       <c r="C6">
-        <v>0.06850000000000001</v>
+        <v>0.1805</v>
       </c>
       <c r="D6">
-        <v>0.0441</v>
+        <v>0.1162</v>
       </c>
       <c r="E6">
-        <v>0.3282999992370605</v>
+        <v>0.8651999831199646</v>
       </c>
       <c r="F6">
-        <v>-0.05119999870657921</v>
+        <v>-0.1348000019788742</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -544,19 +544,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>65.66690063476562</v>
+        <v>173.0357971191406</v>
       </c>
       <c r="C7">
-        <v>0.06610000000000001</v>
+        <v>0.1743</v>
       </c>
       <c r="D7">
-        <v>0.05990000069141388</v>
+        <v>0.1578000038862228</v>
       </c>
       <c r="E7">
-        <v>0.221000000834465</v>
+        <v>0.5821999907493591</v>
       </c>
       <c r="F7">
-        <v>-0.05119999870657921</v>
+        <v>-0.1348000019788742</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -564,19 +564,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>98.10030364990234</v>
+        <v>258.4993896484375</v>
       </c>
       <c r="C8">
-        <v>0.08790000000000001</v>
+        <v>0.2316</v>
       </c>
       <c r="D8">
-        <v>0.08019999999999999</v>
+        <v>0.2115</v>
       </c>
       <c r="E8">
-        <v>0.221000000834465</v>
+        <v>0.5821999907493591</v>
       </c>
       <c r="F8">
-        <v>-0.05119999870657921</v>
+        <v>-0.1348000019788742</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -584,19 +584,19 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>142.3435974121094</v>
+        <v>375.0837097167969</v>
       </c>
       <c r="C9">
-        <v>0.0182</v>
+        <v>0.048</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.3282999992370605</v>
+        <v>0.8651999831199646</v>
       </c>
       <c r="F9">
-        <v>-0.05119999870657921</v>
+        <v>-0.1348000019788742</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
electromagnetic break design update
</commit_message>
<xml_diff>
--- a/new_modules/Summary_2022-06-09_L1C.xlsx
+++ b/new_modules/Summary_2022-06-09_L1C.xlsx
@@ -444,19 +444,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>1298.24462890625</v>
+        <v>1116.312744140625</v>
       </c>
       <c r="C2">
-        <v>0.9739</v>
+        <v>0.8374</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.9006000161170959</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0.3619000017642975</v>
+        <v>0.4099999964237213</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -464,10 +464,10 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>1237.009155273438</v>
+        <v>1208.818115234375</v>
       </c>
       <c r="C3">
-        <v>0.9896</v>
+        <v>0.9671</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -476,7 +476,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>0.5360999703407288</v>
+        <v>0.7092000246047974</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -484,19 +484,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>855.1016845703125</v>
+        <v>813.9815063476562</v>
       </c>
       <c r="C4">
-        <v>0.999</v>
+        <v>0.9509</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0.9804</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0.6179999709129333</v>
+        <v>0.6880999803543091</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -504,19 +504,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>689.8421020507812</v>
+        <v>747.32958984375</v>
       </c>
       <c r="C5">
-        <v>0.7277</v>
+        <v>0.7883</v>
       </c>
       <c r="D5">
-        <v>0.6954</v>
+        <v>0.7813</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.1772000044584274</v>
+        <v>0.5238000154495239</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -524,19 +524,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>865.3720092773438</v>
+        <v>971.8284912109375</v>
       </c>
       <c r="C6">
-        <v>0.6846</v>
+        <v>0.7689</v>
       </c>
       <c r="D6">
-        <v>0.749</v>
+        <v>0.7695</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -544,19 +544,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>686.0853881835938</v>
+        <v>750.70458984375</v>
       </c>
       <c r="C7">
-        <v>0.6909</v>
+        <v>0.756</v>
       </c>
       <c r="D7">
-        <v>0.7073000073432922</v>
+        <v>0.7630000114440918</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>0.2829000055789948</v>
+        <v>0.5792000293731689</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -564,19 +564,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>707.03857421875</v>
+        <v>766.736572265625</v>
       </c>
       <c r="C8">
-        <v>0.6335</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="D8">
-        <v>0.6536999999999999</v>
+        <v>0.6703</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0.9742000102996826</v>
       </c>
       <c r="F8">
-        <v>0.2829000055789948</v>
+        <v>0.5792000293731689</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -584,19 +584,19 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>6338.693359375</v>
+        <v>6375.7119140625</v>
       </c>
       <c r="C9">
-        <v>0.8172</v>
+        <v>0.8218</v>
       </c>
       <c r="D9">
-        <v>0.8652</v>
+        <v>0.8110000000000001</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.4099999964237213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>